<commit_message>
Reverse Theta sign (breaking change) to follow convention of raw derivative
</commit_message>
<xml_diff>
--- a/QuantSharp.Tests/Test cases.xlsx
+++ b/QuantSharp.Tests/Test cases.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E664E8-6DD8-4D51-8F9B-40D1C5C35C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD658CC-575B-4EC5-B6E2-9D7D231EF6B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E6178247-95C5-4BE5-9980-5CAA8CAAD23B}"/>
   </bookViews>
@@ -245,25 +245,25 @@
     <tableColumn id="12" xr3:uid="{975F6A73-1C48-4CF7-838B-0166F12FDBE3}" name="Gamma" dataDxfId="7">
       <calculatedColumnFormula>_xlfn.NORM.S.DIST(Table1[[#This Row],[dPlus]],FALSE) / (Table1[[#This Row],[Underlying]] * Table1[[#This Row],[Sigma]] * SQRT(Table1[[#This Row],[TTE]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{091EE3BC-052D-41CE-BCAA-34164BC60B3C}" name="Theta CALL" dataDxfId="6">
-      <calculatedColumnFormula>-Table1[[#This Row],[Underlying]] * _xlfn.NORM.S.DIST(Table1[[#This Row],[dPlus]],FALSE) * Table1[[#This Row],[Sigma]] / 2 / SQRT(Table1[[#This Row],[TTE]]) - Table1[[#This Row],[Rate]] * Table1[[#This Row],[Strike]] * EXP(-Table1[[#This Row],[Rate]] * Table1[[#This Row],[TTE]]) * _xlfn.NORM.S.DIST(Table1[[#This Row],[dMinus]],TRUE)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="14" xr3:uid="{7F6D6F6B-8B45-4E71-93C9-0696DD761532}" name="Theta PUT" dataDxfId="5">
-      <calculatedColumnFormula>-Table1[[#This Row],[Underlying]] * _xlfn.NORM.S.DIST(Table1[[#This Row],[dPlus]],FALSE) * Table1[[#This Row],[Sigma]] / 2 / SQRT(Table1[[#This Row],[TTE]]) + Table1[[#This Row],[Rate]] * Table1[[#This Row],[Strike]] * EXP(-Table1[[#This Row],[Rate]] * Table1[[#This Row],[TTE]]) * _xlfn.NORM.S.DIST(-Table1[[#This Row],[dMinus]],TRUE)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="15" xr3:uid="{B77019EB-BA05-480F-AAD3-2146850DF83E}" name="Vega" dataDxfId="4">
+    <tableColumn id="13" xr3:uid="{091EE3BC-052D-41CE-BCAA-34164BC60B3C}" name="Theta CALL" dataDxfId="1">
+      <calculatedColumnFormula>Table1[[#This Row],[Underlying]] * _xlfn.NORM.S.DIST(Table1[[#This Row],[dPlus]],FALSE) * Table1[[#This Row],[Sigma]] / 2 / SQRT(Table1[[#This Row],[TTE]]) + Table1[[#This Row],[Rate]] * Table1[[#This Row],[Strike]] * EXP(-Table1[[#This Row],[Rate]] * Table1[[#This Row],[TTE]]) * _xlfn.NORM.S.DIST(Table1[[#This Row],[dMinus]],TRUE)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="14" xr3:uid="{7F6D6F6B-8B45-4E71-93C9-0696DD761532}" name="Theta PUT" dataDxfId="0">
+      <calculatedColumnFormula>Table1[[#This Row],[Underlying]] * _xlfn.NORM.S.DIST(Table1[[#This Row],[dPlus]],FALSE) * Table1[[#This Row],[Sigma]] / 2 / SQRT(Table1[[#This Row],[TTE]]) - Table1[[#This Row],[Rate]] * Table1[[#This Row],[Strike]] * EXP(-Table1[[#This Row],[Rate]] * Table1[[#This Row],[TTE]]) * _xlfn.NORM.S.DIST(-Table1[[#This Row],[dMinus]],TRUE)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="15" xr3:uid="{B77019EB-BA05-480F-AAD3-2146850DF83E}" name="Vega" dataDxfId="6">
       <calculatedColumnFormula>Table1[[#This Row],[Underlying]] * _xlfn.NORM.S.DIST(Table1[[#This Row],[dPlus]],FALSE) * SQRT(Table1[[#This Row],[TTE]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{1A817639-FC4A-4F91-A692-E1278565DCEA}" name="Vomma" dataDxfId="3">
+    <tableColumn id="16" xr3:uid="{1A817639-FC4A-4F91-A692-E1278565DCEA}" name="Vomma" dataDxfId="5">
       <calculatedColumnFormula>Table1[[#This Row],[Vega]] * Table1[[#This Row],[dPlus]] * Table1[[#This Row],[dMinus]] / Table1[[#This Row],[Sigma]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{81A2143B-84B9-4350-87EB-2F8966CEE164}" name="Rho CALL" dataDxfId="2">
+    <tableColumn id="17" xr3:uid="{81A2143B-84B9-4350-87EB-2F8966CEE164}" name="Rho CALL" dataDxfId="4">
       <calculatedColumnFormula>Table1[[#This Row],[Strike]] * Table1[[#This Row],[TTE]] * EXP(-Table1[[#This Row],[Rate]] * Table1[[#This Row],[TTE]]) * _xlfn.NORM.S.DIST(Table1[[#This Row],[dMinus]],TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{D92B5C9A-D9B3-47EB-9D9D-0FDA8A58DECD}" name="Rho PUT" dataDxfId="1">
+    <tableColumn id="18" xr3:uid="{D92B5C9A-D9B3-47EB-9D9D-0FDA8A58DECD}" name="Rho PUT" dataDxfId="3">
       <calculatedColumnFormula>-Table1[[#This Row],[Strike]] * Table1[[#This Row],[TTE]] * EXP(-Table1[[#This Row],[Rate]] * Table1[[#This Row],[TTE]]) * _xlfn.NORM.S.DIST(-Table1[[#This Row],[dMinus]],TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{06954A86-7A31-4C0C-AA30-E4E8B24F8FE5}" name="Test case values" dataDxfId="0">
+    <tableColumn id="19" xr3:uid="{06954A86-7A31-4C0C-AA30-E4E8B24F8FE5}" name="Test case values" dataDxfId="2">
       <calculatedColumnFormula array="1" xml:space="preserve">
 PropBuild("Call",Table1[[#This Row],[CALL]]) &amp;
 PropBuild("Put",Table1[[#This Row],[PUT]]) &amp;
@@ -582,7 +582,7 @@
   <dimension ref="B2:T7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,12 +710,12 @@
         <v>1.37979413657528E-5</v>
       </c>
       <c r="N3">
-        <f>-Table1[[#This Row],[Underlying]] * _xlfn.NORM.S.DIST(Table1[[#This Row],[dPlus]],FALSE) * Table1[[#This Row],[Sigma]] / 2 / SQRT(Table1[[#This Row],[TTE]]) - Table1[[#This Row],[Rate]] * Table1[[#This Row],[Strike]] * EXP(-Table1[[#This Row],[Rate]] * Table1[[#This Row],[TTE]]) * _xlfn.NORM.S.DIST(Table1[[#This Row],[dMinus]],TRUE)</f>
-        <v>-11908.902818069062</v>
+        <f>Table1[[#This Row],[Underlying]] * _xlfn.NORM.S.DIST(Table1[[#This Row],[dPlus]],FALSE) * Table1[[#This Row],[Sigma]] / 2 / SQRT(Table1[[#This Row],[TTE]]) + Table1[[#This Row],[Rate]] * Table1[[#This Row],[Strike]] * EXP(-Table1[[#This Row],[Rate]] * Table1[[#This Row],[TTE]]) * _xlfn.NORM.S.DIST(Table1[[#This Row],[dMinus]],TRUE)</f>
+        <v>11908.902818069062</v>
       </c>
       <c r="O3">
-        <f>-Table1[[#This Row],[Underlying]] * _xlfn.NORM.S.DIST(Table1[[#This Row],[dPlus]],FALSE) * Table1[[#This Row],[Sigma]] / 2 / SQRT(Table1[[#This Row],[TTE]]) + Table1[[#This Row],[Rate]] * Table1[[#This Row],[Strike]] * EXP(-Table1[[#This Row],[Rate]] * Table1[[#This Row],[TTE]]) * _xlfn.NORM.S.DIST(-Table1[[#This Row],[dMinus]],TRUE)</f>
-        <v>-8787.9110995783976</v>
+        <f>Table1[[#This Row],[Underlying]] * _xlfn.NORM.S.DIST(Table1[[#This Row],[dPlus]],FALSE) * Table1[[#This Row],[Sigma]] / 2 / SQRT(Table1[[#This Row],[TTE]]) - Table1[[#This Row],[Rate]] * Table1[[#This Row],[Strike]] * EXP(-Table1[[#This Row],[Rate]] * Table1[[#This Row],[TTE]]) * _xlfn.NORM.S.DIST(-Table1[[#This Row],[dMinus]],TRUE)</f>
+        <v>8787.9110995783976</v>
       </c>
       <c r="P3">
         <f>Table1[[#This Row],[Underlying]] * _xlfn.NORM.S.DIST(Table1[[#This Row],[dPlus]],FALSE) * SQRT(Table1[[#This Row],[TTE]])</f>
@@ -751,8 +751,8 @@
 CallDelta = 0.620807,
 PutDelta = -0.37919,
 Gamma = 1.379794,
-CallTheta = -11908.9,
-PutTheta = -8787.91,
+CallTheta = 11908.90,
+PutTheta = 8787.911,
 Vega = 17488.89,
 Vomma = -1045.99,
 CallRho = 14155.68,
@@ -805,12 +805,12 @@
         <v>1.6175565326817357E-2</v>
       </c>
       <c r="N4">
-        <f>-Table1[[#This Row],[Underlying]] * _xlfn.NORM.S.DIST(Table1[[#This Row],[dPlus]],FALSE) * Table1[[#This Row],[Sigma]] / 2 / SQRT(Table1[[#This Row],[TTE]]) - Table1[[#This Row],[Rate]] * Table1[[#This Row],[Strike]] * EXP(-Table1[[#This Row],[Rate]] * Table1[[#This Row],[TTE]]) * _xlfn.NORM.S.DIST(Table1[[#This Row],[dMinus]],TRUE)</f>
-        <v>-5.0027604455409875</v>
+        <f>Table1[[#This Row],[Underlying]] * _xlfn.NORM.S.DIST(Table1[[#This Row],[dPlus]],FALSE) * Table1[[#This Row],[Sigma]] / 2 / SQRT(Table1[[#This Row],[TTE]]) + Table1[[#This Row],[Rate]] * Table1[[#This Row],[Strike]] * EXP(-Table1[[#This Row],[Rate]] * Table1[[#This Row],[TTE]]) * _xlfn.NORM.S.DIST(Table1[[#This Row],[dMinus]],TRUE)</f>
+        <v>5.0027604455409875</v>
       </c>
       <c r="O4">
-        <f>-Table1[[#This Row],[Underlying]] * _xlfn.NORM.S.DIST(Table1[[#This Row],[dPlus]],FALSE) * Table1[[#This Row],[Sigma]] / 2 / SQRT(Table1[[#This Row],[TTE]]) + Table1[[#This Row],[Rate]] * Table1[[#This Row],[Strike]] * EXP(-Table1[[#This Row],[Rate]] * Table1[[#This Row],[TTE]]) * _xlfn.NORM.S.DIST(-Table1[[#This Row],[dMinus]],TRUE)</f>
-        <v>-4.209462183761711</v>
+        <f>Table1[[#This Row],[Underlying]] * _xlfn.NORM.S.DIST(Table1[[#This Row],[dPlus]],FALSE) * Table1[[#This Row],[Sigma]] / 2 / SQRT(Table1[[#This Row],[TTE]]) - Table1[[#This Row],[Rate]] * Table1[[#This Row],[Strike]] * EXP(-Table1[[#This Row],[Rate]] * Table1[[#This Row],[TTE]]) * _xlfn.NORM.S.DIST(-Table1[[#This Row],[dMinus]],TRUE)</f>
+        <v>4.209462183761711</v>
       </c>
       <c r="P4">
         <f>Table1[[#This Row],[Underlying]] * _xlfn.NORM.S.DIST(Table1[[#This Row],[dPlus]],FALSE) * SQRT(Table1[[#This Row],[TTE]])</f>
@@ -846,8 +846,8 @@
 CallDelta = 0.592313,
 PutDelta = -0.40768,
 Gamma = 0.016175,
-CallTheta = -5.00276,
-PutTheta = -4.20946,
+CallTheta = 5.002760,
+PutTheta = 4.209462,
 Vega = 23.29281,
 Vomma = -2.26393,
 CallRho = 25.68639,
@@ -900,12 +900,12 @@
         <v>4.2152222727056103E-5</v>
       </c>
       <c r="N5">
-        <f>-Table1[[#This Row],[Underlying]] * _xlfn.NORM.S.DIST(Table1[[#This Row],[dPlus]],FALSE) * Table1[[#This Row],[Sigma]] / 2 / SQRT(Table1[[#This Row],[TTE]]) - Table1[[#This Row],[Rate]] * Table1[[#This Row],[Strike]] * EXP(-Table1[[#This Row],[Rate]] * Table1[[#This Row],[TTE]]) * _xlfn.NORM.S.DIST(Table1[[#This Row],[dMinus]],TRUE)</f>
-        <v>-303.4448071576337</v>
+        <f>Table1[[#This Row],[Underlying]] * _xlfn.NORM.S.DIST(Table1[[#This Row],[dPlus]],FALSE) * Table1[[#This Row],[Sigma]] / 2 / SQRT(Table1[[#This Row],[TTE]]) + Table1[[#This Row],[Rate]] * Table1[[#This Row],[Strike]] * EXP(-Table1[[#This Row],[Rate]] * Table1[[#This Row],[TTE]]) * _xlfn.NORM.S.DIST(Table1[[#This Row],[dMinus]],TRUE)</f>
+        <v>303.4448071576337</v>
       </c>
       <c r="O5">
-        <f>-Table1[[#This Row],[Underlying]] * _xlfn.NORM.S.DIST(Table1[[#This Row],[dPlus]],FALSE) * Table1[[#This Row],[Sigma]] / 2 / SQRT(Table1[[#This Row],[TTE]]) + Table1[[#This Row],[Rate]] * Table1[[#This Row],[Strike]] * EXP(-Table1[[#This Row],[Rate]] * Table1[[#This Row],[TTE]]) * _xlfn.NORM.S.DIST(-Table1[[#This Row],[dMinus]],TRUE)</f>
-        <v>-257.67423311477029</v>
+        <f>Table1[[#This Row],[Underlying]] * _xlfn.NORM.S.DIST(Table1[[#This Row],[dPlus]],FALSE) * Table1[[#This Row],[Sigma]] / 2 / SQRT(Table1[[#This Row],[TTE]]) - Table1[[#This Row],[Rate]] * Table1[[#This Row],[Strike]] * EXP(-Table1[[#This Row],[Rate]] * Table1[[#This Row],[TTE]]) * _xlfn.NORM.S.DIST(-Table1[[#This Row],[dMinus]],TRUE)</f>
+        <v>257.67423311477029</v>
       </c>
       <c r="P5">
         <f>Table1[[#This Row],[Underlying]] * _xlfn.NORM.S.DIST(Table1[[#This Row],[dPlus]],FALSE) * SQRT(Table1[[#This Row],[TTE]])</f>
@@ -941,8 +941,8 @@
 CallDelta = 0.966690,
 PutDelta = -0.03330,
 Gamma = 4.215222,
-CallTheta = -303.444,
-PutTheta = -257.674,
+CallTheta = 303.4448,
+PutTheta = 257.6742,
 Vega = 163.2134,
 Vomma = 536.7141,
 CallRho = 528.7919,
@@ -995,12 +995,12 @@
         <v>1.1473779493236266E-3</v>
       </c>
       <c r="N6">
-        <f>-Table1[[#This Row],[Underlying]] * _xlfn.NORM.S.DIST(Table1[[#This Row],[dPlus]],FALSE) * Table1[[#This Row],[Sigma]] / 2 / SQRT(Table1[[#This Row],[TTE]]) - Table1[[#This Row],[Rate]] * Table1[[#This Row],[Strike]] * EXP(-Table1[[#This Row],[Rate]] * Table1[[#This Row],[TTE]]) * _xlfn.NORM.S.DIST(Table1[[#This Row],[dMinus]],TRUE)</f>
-        <v>-7.1653211975417586</v>
+        <f>Table1[[#This Row],[Underlying]] * _xlfn.NORM.S.DIST(Table1[[#This Row],[dPlus]],FALSE) * Table1[[#This Row],[Sigma]] / 2 / SQRT(Table1[[#This Row],[TTE]]) + Table1[[#This Row],[Rate]] * Table1[[#This Row],[Strike]] * EXP(-Table1[[#This Row],[Rate]] * Table1[[#This Row],[TTE]]) * _xlfn.NORM.S.DIST(Table1[[#This Row],[dMinus]],TRUE)</f>
+        <v>7.1653211975417586</v>
       </c>
       <c r="O6">
-        <f>-Table1[[#This Row],[Underlying]] * _xlfn.NORM.S.DIST(Table1[[#This Row],[dPlus]],FALSE) * Table1[[#This Row],[Sigma]] / 2 / SQRT(Table1[[#This Row],[TTE]]) + Table1[[#This Row],[Rate]] * Table1[[#This Row],[Strike]] * EXP(-Table1[[#This Row],[Rate]] * Table1[[#This Row],[TTE]]) * _xlfn.NORM.S.DIST(-Table1[[#This Row],[dMinus]],TRUE)</f>
-        <v>-2.1778055855544585</v>
+        <f>Table1[[#This Row],[Underlying]] * _xlfn.NORM.S.DIST(Table1[[#This Row],[dPlus]],FALSE) * Table1[[#This Row],[Sigma]] / 2 / SQRT(Table1[[#This Row],[TTE]]) - Table1[[#This Row],[Rate]] * Table1[[#This Row],[Strike]] * EXP(-Table1[[#This Row],[Rate]] * Table1[[#This Row],[TTE]]) * _xlfn.NORM.S.DIST(-Table1[[#This Row],[dMinus]],TRUE)</f>
+        <v>2.1778055855544585</v>
       </c>
       <c r="P6">
         <f>Table1[[#This Row],[Underlying]] * _xlfn.NORM.S.DIST(Table1[[#This Row],[dPlus]],FALSE) * SQRT(Table1[[#This Row],[TTE]])</f>
@@ -1036,8 +1036,8 @@
 CallDelta = 0.027701,
 PutDelta = -0.97229,
 Gamma = 0.001147,
-CallTheta = -7.16532,
-PutTheta = -2.17780,
+CallTheta = 7.165321,
+PutTheta = 2.177805,
 Vega = 11.78070,
 Vomma = 155.3978,
 CallRho = 2.422483,
@@ -1090,12 +1090,12 @@
         <v>1.25217817396271E-2</v>
       </c>
       <c r="N7">
-        <f>-Table1[[#This Row],[Underlying]] * _xlfn.NORM.S.DIST(Table1[[#This Row],[dPlus]],FALSE) * Table1[[#This Row],[Sigma]] / 2 / SQRT(Table1[[#This Row],[TTE]]) - Table1[[#This Row],[Rate]] * Table1[[#This Row],[Strike]] * EXP(-Table1[[#This Row],[Rate]] * Table1[[#This Row],[TTE]]) * _xlfn.NORM.S.DIST(Table1[[#This Row],[dMinus]],TRUE)</f>
-        <v>-20.920447135550365</v>
+        <f>Table1[[#This Row],[Underlying]] * _xlfn.NORM.S.DIST(Table1[[#This Row],[dPlus]],FALSE) * Table1[[#This Row],[Sigma]] / 2 / SQRT(Table1[[#This Row],[TTE]]) + Table1[[#This Row],[Rate]] * Table1[[#This Row],[Strike]] * EXP(-Table1[[#This Row],[Rate]] * Table1[[#This Row],[TTE]]) * _xlfn.NORM.S.DIST(Table1[[#This Row],[dMinus]],TRUE)</f>
+        <v>20.920447135550365</v>
       </c>
       <c r="O7">
-        <f>-Table1[[#This Row],[Underlying]] * _xlfn.NORM.S.DIST(Table1[[#This Row],[dPlus]],FALSE) * Table1[[#This Row],[Sigma]] / 2 / SQRT(Table1[[#This Row],[TTE]]) + Table1[[#This Row],[Rate]] * Table1[[#This Row],[Strike]] * EXP(-Table1[[#This Row],[Rate]] * Table1[[#This Row],[TTE]]) * _xlfn.NORM.S.DIST(-Table1[[#This Row],[dMinus]],TRUE)</f>
-        <v>0.36564334566141765</v>
+        <f>Table1[[#This Row],[Underlying]] * _xlfn.NORM.S.DIST(Table1[[#This Row],[dPlus]],FALSE) * Table1[[#This Row],[Sigma]] / 2 / SQRT(Table1[[#This Row],[TTE]]) - Table1[[#This Row],[Rate]] * Table1[[#This Row],[Strike]] * EXP(-Table1[[#This Row],[Rate]] * Table1[[#This Row],[TTE]]) * _xlfn.NORM.S.DIST(-Table1[[#This Row],[dMinus]],TRUE)</f>
+        <v>-0.36564334566141765</v>
       </c>
       <c r="P7">
         <f>Table1[[#This Row],[Underlying]] * _xlfn.NORM.S.DIST(Table1[[#This Row],[dPlus]],FALSE) * SQRT(Table1[[#This Row],[TTE]])</f>
@@ -1131,8 +1131,8 @@
 CallDelta = 0.928278,
 PutDelta = -0.07172,
 Gamma = 0.012521,
-CallTheta = -20.9204,
-PutTheta = 0.365643,
+CallTheta = 20.92044,
+PutTheta = -0.36564,
 Vega = 9.963268,
 Vomma = 131.8764,
 CallRho = 40.47074,

</xml_diff>